<commit_message>
completed Vehicle Master Data
</commit_message>
<xml_diff>
--- a/template/Vehicle_Template.xlsx
+++ b/template/Vehicle_Template.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="28526"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="28827"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\jihbi\xampp\htdocs\synctronix\template\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\xampp\htdocs\synctronix\template\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{07FD3096-85FC-4B05-A1F3-4668024F1EB1}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3833C6ED-C4EC-43D7-BF89-68023617929D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="45" yWindow="-16320" windowWidth="29040" windowHeight="15720" xr2:uid="{9341FD95-CFC6-421C-9B6B-E00C8B5A4387}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{9341FD95-CFC6-421C-9B6B-E00C8B5A4387}"/>
   </bookViews>
   <sheets>
     <sheet name="customermaster" sheetId="1" r:id="rId1"/>
@@ -25,19 +25,19 @@
     <t>Vehicle No</t>
   </si>
   <si>
-    <t>Transporter Code</t>
-  </si>
-  <si>
-    <t>Transporter Name</t>
-  </si>
-  <si>
     <t>Customer Name</t>
   </si>
   <si>
     <t>Customer Code</t>
   </si>
   <si>
-    <t>Ex-Quarry/Delivered</t>
+    <t>Supplier Code</t>
+  </si>
+  <si>
+    <t>Supplier Name</t>
+  </si>
+  <si>
+    <t>Vehicle Weight (KG)</t>
   </si>
 </sst>
 </file>
@@ -400,37 +400,35 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{7E7AE52E-5E3F-4816-BCAD-C318F36103B6}">
-  <dimension ref="A1:T1"/>
+  <dimension ref="A1:R1"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B2" sqref="B2"/>
+      <selection activeCell="H14" sqref="H14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="16.42578125" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="19.7109375" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="16.42578125" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="17.28515625" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="14.7109375" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="15.42578125" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="25.28515625" style="3" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="14" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="12.140625" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="27.7109375" style="3" bestFit="1" customWidth="1"/>
-    <col min="11" max="11" width="14.5703125" bestFit="1" customWidth="1"/>
-    <col min="12" max="12" width="14.42578125" bestFit="1" customWidth="1"/>
-    <col min="13" max="13" width="16.42578125" bestFit="1" customWidth="1"/>
-    <col min="14" max="14" width="17.28515625" bestFit="1" customWidth="1"/>
-    <col min="15" max="15" width="15.85546875" bestFit="1" customWidth="1"/>
-    <col min="16" max="16" width="12.85546875" bestFit="1" customWidth="1"/>
-    <col min="17" max="17" width="13.7109375" bestFit="1" customWidth="1"/>
-    <col min="18" max="18" width="10.7109375" bestFit="1" customWidth="1"/>
-    <col min="19" max="19" width="14.42578125" bestFit="1" customWidth="1"/>
-    <col min="20" max="20" width="8.5703125" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="16.42578125" customWidth="1"/>
+    <col min="3" max="3" width="14.7109375" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="15.42578125" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="14.7109375" style="3" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="14" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="12.140625" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="27.7109375" style="3" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="14.5703125" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="14.42578125" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="16.42578125" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="17.28515625" bestFit="1" customWidth="1"/>
+    <col min="13" max="13" width="15.85546875" bestFit="1" customWidth="1"/>
+    <col min="14" max="14" width="12.85546875" bestFit="1" customWidth="1"/>
+    <col min="15" max="15" width="13.7109375" bestFit="1" customWidth="1"/>
+    <col min="16" max="16" width="10.7109375" bestFit="1" customWidth="1"/>
+    <col min="17" max="17" width="14.42578125" bestFit="1" customWidth="1"/>
+    <col min="18" max="18" width="8.5703125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:20" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -438,21 +436,21 @@
         <v>5</v>
       </c>
       <c r="C1" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="D1" s="1" t="s">
         <v>1</v>
       </c>
-      <c r="D1" s="1" t="s">
-        <v>2</v>
-      </c>
       <c r="E1" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="F1" s="1" t="s">
         <v>4</v>
       </c>
-      <c r="F1" s="1" t="s">
-        <v>3</v>
-      </c>
-      <c r="G1" s="2"/>
-      <c r="H1" s="1"/>
+      <c r="G1" s="1"/>
+      <c r="H1" s="2"/>
       <c r="I1" s="1"/>
-      <c r="J1" s="2"/>
+      <c r="J1" s="1"/>
       <c r="K1" s="1"/>
       <c r="L1" s="1"/>
       <c r="M1" s="1"/>
@@ -461,15 +459,8 @@
       <c r="P1" s="1"/>
       <c r="Q1" s="1"/>
       <c r="R1" s="1"/>
-      <c r="S1" s="1"/>
-      <c r="T1" s="1"/>
     </row>
   </sheetData>
-  <dataValidations count="1">
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="B2:B1048576" xr:uid="{12D1E684-0453-4180-A718-6436A71F3A78}">
-      <formula1>"Ex-Quarry, Delivered"</formula1>
-    </dataValidation>
-  </dataValidations>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
 </worksheet>
 </file>
</xml_diff>